<commit_message>
DataProvider added to BaseTest. Login Tests added
</commit_message>
<xml_diff>
--- a/CapstoneProject/Resources/data/TestData.xlsx
+++ b/CapstoneProject/Resources/data/TestData.xlsx
@@ -5,14 +5,14 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDET\Codeprojects\SDETHomework\MMC_SeleniumAutomation\TestAutomation\Resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDET\Codeprojects\SDETHomework\Team1_OrangeHRM\CapstoneProject\Resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5600"/>
   </bookViews>
   <sheets>
-    <sheet name="Valid" sheetId="1" r:id="rId1"/>
+    <sheet name="testValidAdminLogin" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -362,7 +362,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Login Tests and PIM Tests added.
</commit_message>
<xml_diff>
--- a/CapstoneProject/Resources/data/TestData.xlsx
+++ b/CapstoneProject/Resources/data/TestData.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="testValidAdminLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="testInvalidAdminLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="testPIMPageLinks" sheetId="3" r:id="rId3"/>
+    <sheet name="testCreateUser" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -41,6 +42,36 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>invalidUserName</t>
+  </si>
+  <si>
+    <t>invalidPassword</t>
+  </si>
+  <si>
+    <t>TabNames</t>
+  </si>
+  <si>
+    <t>Employee List;Add Employee;Reports</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Potter</t>
   </si>
 </sst>
 </file>
@@ -361,8 +392,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -402,14 +433,31 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -417,12 +465,86 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added claim testcase with testdata sheet
</commit_message>
<xml_diff>
--- a/CapstoneProject/Resources/data/TestData.xlsx
+++ b/CapstoneProject/Resources/data/TestData.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDET\Codeprojects\SDETHomework\Team1_OrangeHRM\CapstoneProject\Resources\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5600" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14010" windowHeight="4170" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="testValidAdminLogin" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,11 @@
     <sheet name="testPIMPageLinks" sheetId="3" r:id="rId3"/>
     <sheet name="testCreateUser" sheetId="4" r:id="rId4"/>
     <sheet name="testDashboardSections" sheetId="5" r:id="rId5"/>
+    <sheet name="testCreateClaim" sheetId="6" r:id="rId6"/>
+    <sheet name="testCancelclaim" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:N12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -79,6 +77,18 @@
   </si>
   <si>
     <t>Time at Work;My Actions;Quick Launch;Buzz Latest Posts;Employees on Leave Today;Employee Distribution by Sub Unit;Employee Distribution by Location</t>
+  </si>
+  <si>
+    <t>Event_select</t>
+  </si>
+  <si>
+    <t>Currency_select</t>
+  </si>
+  <si>
+    <t>Travel Allowance</t>
+  </si>
+  <si>
+    <t>Afghanistan Afghani</t>
   </si>
 </sst>
 </file>
@@ -401,12 +411,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -435,6 +445,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -449,8 +460,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -471,6 +482,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -509,6 +521,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -558,6 +571,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -565,11 +579,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
@@ -598,5 +612,94 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added dashboard claims testcase for claimns
</commit_message>
<xml_diff>
--- a/CapstoneProject/Resources/data/TestData.xlsx
+++ b/CapstoneProject/Resources/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14010" windowHeight="4170" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21140" windowHeight="9480" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="testValidAdminLogin" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,10 @@
     <sheet name="testDashboardSections" sheetId="5" r:id="rId5"/>
     <sheet name="testCreateClaim" sheetId="6" r:id="rId6"/>
     <sheet name="testCancelclaim" sheetId="7" r:id="rId7"/>
+    <sheet name="testClaimDashboard" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N12"/>
+  <oleSize ref="A1:U30"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Username</t>
   </si>
@@ -89,6 +90,30 @@
   </si>
   <si>
     <t>Afghanistan Afghani</t>
+  </si>
+  <si>
+    <t>Header1</t>
+  </si>
+  <si>
+    <t>Header2</t>
+  </si>
+  <si>
+    <t>Header3</t>
+  </si>
+  <si>
+    <t>Header4</t>
+  </si>
+  <si>
+    <t>Submit Claim</t>
+  </si>
+  <si>
+    <t>My Claims</t>
+  </si>
+  <si>
+    <t>Employee Claims</t>
+  </si>
+  <si>
+    <t>Assign Claim</t>
   </si>
 </sst>
 </file>
@@ -664,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -702,4 +727,63 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
RecruitmentPage updated and 2 Recruitment TestCases added
</commit_message>
<xml_diff>
--- a/CapstoneProject/Resources/data/TestData.xlsx
+++ b/CapstoneProject/Resources/data/TestData.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDET\Codeprojects\SDETHomework\Team1_OrangeHRM\CapstoneProject\Resources\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21140" windowHeight="9480" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21140" windowHeight="9480" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="testValidAdminLogin" sheetId="1" r:id="rId1"/>
@@ -15,9 +20,10 @@
     <sheet name="testCreateClaim" sheetId="6" r:id="rId6"/>
     <sheet name="testCancelclaim" sheetId="7" r:id="rId7"/>
     <sheet name="testClaimDashboard" sheetId="8" r:id="rId8"/>
+    <sheet name="testCreateVacancy" sheetId="9" r:id="rId9"/>
+    <sheet name="testVacancySearch" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:U30"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>Username</t>
   </si>
@@ -114,6 +120,36 @@
   </si>
   <si>
     <t>Assign Claim</t>
+  </si>
+  <si>
+    <t>VacancyName</t>
+  </si>
+  <si>
+    <t>Vacancy for CapstoneProject</t>
+  </si>
+  <si>
+    <t>JobTitle</t>
+  </si>
+  <si>
+    <t>QA Lead</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Automation Tester</t>
+  </si>
+  <si>
+    <t>HiringManager</t>
+  </si>
+  <si>
+    <t>Orange Test</t>
+  </si>
+  <si>
+    <t>NumOfPositions</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -149,9 +185,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,6 +511,37 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
@@ -731,10 +799,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -743,7 +811,7 @@
     <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -763,7 +831,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -781,6 +849,67 @@
       </c>
       <c r="F2" t="s">
         <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RecruitmentPage and Tests added
</commit_message>
<xml_diff>
--- a/CapstoneProject/Resources/data/TestData.xlsx
+++ b/CapstoneProject/Resources/data/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21140" windowHeight="9480" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21140" windowHeight="9480" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="testValidAdminLogin" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="testClaimDashboard" sheetId="8" r:id="rId8"/>
     <sheet name="testCreateVacancy" sheetId="9" r:id="rId9"/>
     <sheet name="testVacancySearch" sheetId="10" r:id="rId10"/>
+    <sheet name="testCreateCandidate" sheetId="11" r:id="rId11"/>
+    <sheet name="testRecruitmentPageTabs" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
   <si>
     <t>Username</t>
   </si>
@@ -150,6 +152,27 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>Ron</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>Weasley</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ron@example.com</t>
+  </si>
+  <si>
+    <t>Tabs</t>
+  </si>
+  <si>
+    <t>Candidates;Vacancies</t>
   </si>
 </sst>
 </file>
@@ -542,6 +565,98 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
@@ -860,7 +975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>

</xml_diff>